<commit_message>
Using the input parameters in excel file, generate a bunch of images which can be used as training dataset.
</commit_message>
<xml_diff>
--- a/main/prepareCropImages.xlsx
+++ b/main/prepareCropImages.xlsx
@@ -194,8 +194,8 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -265,7 +265,7 @@
         <v>25</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +297,7 @@
         <v>25</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +329,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove the cropsize parameter and select new images for training.
</commit_message>
<xml_diff>
--- a/main/prepareCropImages.xlsx
+++ b/main/prepareCropImages.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Input file name and path</t>
   </si>
@@ -44,22 +44,34 @@
     <t xml:space="preserve">Column of the bottom left pillar</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of pillars in the top row</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of pilars in the bottom row</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size of crop image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../datasetForTraining/20kX _0888.dm3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../datasetForTraining/20kX _0889.dm3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../datasetForTraining/20kX _0890.dm3</t>
+    <t xml:space="preserve">Number of pillars in the first row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of pilars in the first column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _0791.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _0792.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _0793.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _0794.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _4066.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _4067.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _4068.dm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../datasetForTraining/20kX _4069.dm3</t>
   </si>
   <si>
     <t xml:space="preserve">/scratch/utkur/utkarsh/RestorePillars/datasetForTraining/20kX _0891.dm3</t>
@@ -192,10 +204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,7 +216,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -232,22 +244,20 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>3960</v>
@@ -256,80 +266,216 @@
         <v>3948</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>25</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>25</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>108</v>
-      </c>
       <c r="D3" s="0" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>3990</v>
+        <v>3954</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>3936</v>
+        <v>3918</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>200</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4002</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3918</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="B5" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3912</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>3918</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>3972</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="H5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>3894</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>3930</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3990</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3930</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>3966</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>200</v>
+      <c r="F8" s="0" t="n">
+        <v>4038</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3978</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>3906</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -361,37 +507,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>